<commit_message>
formatting of value input files
</commit_message>
<xml_diff>
--- a/data/test_inputs/preprocessing/ecology_format/ecology_values_PLA_impeller.xlsx
+++ b/data/test_inputs/preprocessing/ecology_format/ecology_values_PLA_impeller.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/ecology_format/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/test_inputs/preprocessing/ecology_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29E6689-CB9E-8C4F-808F-E5313D480602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0C7959-AB1B-774F-B9C4-9349C2A7664A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5720" yWindow="1040" windowWidth="19980" windowHeight="17440" activeTab="1" xr2:uid="{963D30B2-CFD0-FD4A-A1E5-CBFAB3BB1A2F}"/>
+    <workbookView xWindow="5720" yWindow="1040" windowWidth="19980" windowHeight="17440" xr2:uid="{963D30B2-CFD0-FD4A-A1E5-CBFAB3BB1A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="ecological_params" sheetId="1" r:id="rId1"/>
@@ -40,15 +40,6 @@
     <t>resources</t>
   </si>
   <si>
-    <t>PLA_impellar_virgin_(recipe_endpoint_h)</t>
-  </si>
-  <si>
-    <t>PLA_impellar_recycled_(recipe_endpoint_h)</t>
-  </si>
-  <si>
-    <t>PLA_impellar_recycled_industrial_(recipe_endpoint_h)</t>
-  </si>
-  <si>
     <t>Min</t>
   </si>
   <si>
@@ -56,6 +47,15 @@
   </si>
   <si>
     <t>Inversion</t>
+  </si>
+  <si>
+    <t>PLA_virgin</t>
+  </si>
+  <si>
+    <t>PLA_recycled</t>
+  </si>
+  <si>
+    <t>PLA_recycled_industrial</t>
   </si>
 </sst>
 </file>
@@ -139,9 +139,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -156,6 +153,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1967EC9D-4F84-D54F-B33E-99CA283C210F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,55 +489,55 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
+      <c r="B1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>878.8</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>993.2</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>666.9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>472.4</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>510.4</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>350.7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>820.5</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>925.7</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>488.5</v>
       </c>
     </row>
@@ -552,65 +550,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FA6DE0E-D102-8443-9553-48EFAE40319B}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>9</v>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>300</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>1200</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>300</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>1200</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>300</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>1200</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>